<commit_message>
Check in the first try at soldering up the board
</commit_message>
<xml_diff>
--- a/P1001-001 - 16bit CPU/Dim1001 - 16bit CPU.xlsx
+++ b/P1001-001 - 16bit CPU/Dim1001 - 16bit CPU.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE4651B-0172-4908-9CAF-008762C452BA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A4FE53-EC03-4FBF-B396-8845A3838D52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>mm</t>
   </si>
@@ -49,19 +52,22 @@
     <t>BoardHeight</t>
   </si>
   <si>
-    <t>BaseLength</t>
-  </si>
-  <si>
-    <t>BaseBoardOffset</t>
-  </si>
-  <si>
-    <t>BaseWidth</t>
-  </si>
-  <si>
     <t>HorizOffsetBetweenScrews</t>
   </si>
   <si>
     <t>VertOffsetBetweenScrews</t>
+  </si>
+  <si>
+    <t>Boarder</t>
+  </si>
+  <si>
+    <t>TwoBoardWidth</t>
+  </si>
+  <si>
+    <t>NumberOfRows</t>
+  </si>
+  <si>
+    <t>NumberOfGaps</t>
   </si>
 </sst>
 </file>
@@ -379,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -461,8 +467,8 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <f>2*B8+3*B1+2*B5</f>
-        <v>648</v>
+        <f>B1-B4-B4</f>
+        <v>192</v>
       </c>
       <c r="C7" t="s">
         <v>0</v>
@@ -473,7 +479,8 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>20</v>
+        <f>B2-B4-B4</f>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
@@ -484,8 +491,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <f>2*B8+10*B2+9*B5</f>
-        <v>556</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
@@ -493,14 +499,11 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B10">
-        <f>B2-B4-B4</f>
-        <v>40</v>
-      </c>
-      <c r="C10" t="s">
-        <v>0</v>
+        <f>B11-1</f>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -508,10 +511,30 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <f>B1-B4-B4</f>
-        <v>192</v>
-      </c>
-      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <f>B9+B9+B11*B2+B10*B5</f>
+        <v>556</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <f>B9+B9+B1+B5+B1</f>
+        <v>444</v>
+      </c>
+      <c r="C13" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>